<commit_message>
all in one, spreadsheet update
</commit_message>
<xml_diff>
--- a/strategies.xlsx
+++ b/strategies.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Map1 - Simple" sheetId="1" r:id="rId1"/>
+    <sheet name="Map 1 - Complete" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="267">
   <si>
     <t>dist full x2</t>
   </si>
   <si>
-    <t>Distance strategy alone</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>MIXED STRATEGIES (x2)</t>
   </si>
   <si>
-    <t>Distance vs. Fuel</t>
-  </si>
-  <si>
     <t>1315+12</t>
   </si>
   <si>
@@ -228,9 +222,6 @@
     <t>(0,1)</t>
   </si>
   <si>
-    <t>Distance vs. Damage</t>
-  </si>
-  <si>
     <t>1295+10</t>
   </si>
   <si>
@@ -327,9 +318,6 @@
     <t>MIXED STRATEGIES (x3)</t>
   </si>
   <si>
-    <t>Distance vs. Fuel vs. Damage</t>
-  </si>
-  <si>
     <t>(1-B)*dist + B*dam_full</t>
   </si>
   <si>
@@ -763,6 +751,72 @@
   </si>
   <si>
     <t>604+8</t>
+  </si>
+  <si>
+    <t>Time strategy alone</t>
+  </si>
+  <si>
+    <t>Time vs. Fuel</t>
+  </si>
+  <si>
+    <t>Time vs. Damage</t>
+  </si>
+  <si>
+    <t>Time vs. Fuel vs. Damage</t>
+  </si>
+  <si>
+    <t>1693+11</t>
+  </si>
+  <si>
+    <t>121+5</t>
+  </si>
+  <si>
+    <t>741+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map02: </t>
+  </si>
+  <si>
+    <t>1468+7</t>
+  </si>
+  <si>
+    <t>208+6</t>
+  </si>
+  <si>
+    <t>354+6</t>
+  </si>
+  <si>
+    <t>PurofMovio:</t>
+  </si>
+  <si>
+    <t>AllInOne</t>
+  </si>
+  <si>
+    <t>(X,Y,Z)</t>
+  </si>
+  <si>
+    <t>1724+14</t>
+  </si>
+  <si>
+    <t>127+2</t>
+  </si>
+  <si>
+    <t>793+16</t>
+  </si>
+  <si>
+    <t>3 STRATEGIES WEIGHTED SUM</t>
+  </si>
+  <si>
+    <t>No Pareto Front MCTS</t>
+  </si>
+  <si>
+    <t>1651+82</t>
+  </si>
+  <si>
+    <t>560+7</t>
+  </si>
+  <si>
+    <t>658+17</t>
   </si>
 </sst>
 </file>
@@ -786,7 +840,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,6 +862,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,6 +933,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD30" sqref="AD30"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1264,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1209,29 +1272,29 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -1239,418 +1302,367 @@
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Z2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>118</v>
+        <v>262</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="AC2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="S3" s="3" t="s">
-        <v>70</v>
+        <v>247</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="V3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="Z3" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="W4" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>124</v>
+        <v>70</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="L5" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD5" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE5" s="6" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="V6" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD6" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E8" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="N8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC8" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="AE8" s="6" t="s">
-        <v>137</v>
+        <v>95</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC9" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>140</v>
+        <v>98</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="5"/>
@@ -1658,17 +1670,23 @@
       <c r="V10" s="4"/>
       <c r="W10" s="7"/>
       <c r="X10" s="6"/>
+      <c r="Z10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="AB10" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="AE10" s="6" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -1678,37 +1696,37 @@
       <c r="V11" s="4"/>
       <c r="W11" s="7"/>
       <c r="X11" s="6"/>
-      <c r="AA11" s="1" t="s">
-        <v>144</v>
+      <c r="Z11" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="AB11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AC11" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="AD11" s="5" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="AE11" s="6" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="5"/>
@@ -1717,33 +1735,33 @@
       <c r="W12" s="7"/>
       <c r="X12" s="6"/>
       <c r="AB12" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="AE12" s="6" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="5"/>
@@ -1752,397 +1770,394 @@
       <c r="W13" s="7"/>
       <c r="X13" s="6"/>
       <c r="AB13" s="1" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AE13" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E14" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>40</v>
+      <c r="AA14" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="AD14" s="5" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="AE14" s="6" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F15" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>43</v>
+      <c r="AB15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="F16" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>46</v>
+      <c r="AB16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F17" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>49</v>
+      <c r="AA17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC17" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD17" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F18" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="L18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
-      <c r="Z18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE18" s="2" t="s">
-        <v>4</v>
+      <c r="AB18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC18" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD18" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F19" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="I19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="L19" s="3" t="s">
-        <v>61</v>
+        <v>246</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P19" s="2" t="s">
+      <c r="Q19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q19" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="S19" s="3" t="s">
-        <v>70</v>
+        <v>247</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="V19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="X19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z19" s="3" t="s">
-        <v>103</v>
+      <c r="AB19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC19" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE19" s="6" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L20" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="V20" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="W20" s="7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA20" s="1" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC20" s="9" t="s">
-        <v>199</v>
+        <v>150</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="AE20" s="6" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L21" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="T21" s="1"/>
       <c r="U21" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="W21" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="Z21" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC21" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD21" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="AE21" s="6" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E22" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V22" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="W22" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC22" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="AE22" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="AF22" s="1" t="s">
-        <v>240</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E23" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="X23" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC23" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="AD23" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="AE23" s="6" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
@@ -2151,118 +2166,121 @@
       <c r="C24" s="8"/>
       <c r="D24" s="12"/>
       <c r="E24" s="8" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="W24" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="X24" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AC24" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="AD24" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="AE24" s="11" t="s">
-        <v>215</v>
+        <v>191</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE24" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="N25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="X25" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB25" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AC25" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="AD25" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="AE25" s="11" t="s">
-        <v>218</v>
+        <v>194</v>
+      </c>
+      <c r="Z25" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="O26" s="4"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="7"/>
+      <c r="Z26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="AB26" s="1" t="s">
-        <v>210</v>
+        <v>121</v>
       </c>
       <c r="AC26" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="AD26" s="10" t="s">
-        <v>220</v>
+        <v>195</v>
+      </c>
+      <c r="AD26" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="AE26" s="6" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="O27" s="4"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="7"/>
-      <c r="AA27" s="1" t="s">
-        <v>128</v>
+      <c r="Z27" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC27" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="AD27" s="5" t="s">
-        <v>222</v>
+        <v>122</v>
+      </c>
+      <c r="AC27" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD27" s="10" t="s">
+        <v>199</v>
       </c>
       <c r="AE27" s="6" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
@@ -2270,16 +2288,19 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="7"/>
       <c r="AB28" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="AD28" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="AE28" s="6" t="s">
-        <v>226</v>
+        <v>201</v>
+      </c>
+      <c r="AD28" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE28" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF28" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
@@ -2287,111 +2308,198 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="7"/>
       <c r="AB29" s="1" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AD29" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="AE29" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF29" s="1" t="s">
-        <v>241</v>
+        <v>207</v>
+      </c>
+      <c r="AE29" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AB30" s="1" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="AD30" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE30" s="6" t="s">
-        <v>160</v>
+        <v>209</v>
+      </c>
+      <c r="AD30" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="AE30" s="11" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AB31" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AC31" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD31" s="10" t="s">
-        <v>231</v>
+        <v>205</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD31" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="AE31" s="11" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AB32" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AC32" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD32" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE32" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AA33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD33" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="AE33" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD34" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE34" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC35" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD35" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE35" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF35" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB36" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD36" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE36" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC37" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD37" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE37" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB38" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC38" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AD38" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE38" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB39" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC39" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AD39" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="AD32" s="5" t="s">
+      <c r="AE39" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="AE32" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33" spans="27:31" x14ac:dyDescent="0.25">
-      <c r="AB33" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC33" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="AD33" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="AE33" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="34" spans="27:31" x14ac:dyDescent="0.25">
-      <c r="AA34" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB34" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC34" s="4"/>
-      <c r="AD34" s="5"/>
-      <c r="AE34" s="6"/>
-    </row>
-    <row r="35" spans="27:31" x14ac:dyDescent="0.25">
-      <c r="AB35" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC35" s="4"/>
-      <c r="AD35" s="5"/>
-      <c r="AE35" s="6"/>
-    </row>
-    <row r="36" spans="27:31" x14ac:dyDescent="0.25">
-      <c r="AB36" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC36" s="4"/>
-      <c r="AD36" s="5"/>
-      <c r="AE36" s="6"/>
-    </row>
-    <row r="37" spans="27:31" x14ac:dyDescent="0.25">
-      <c r="AB37" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC37" s="4"/>
-      <c r="AD37" s="5"/>
-      <c r="AE37" s="6"/>
+    </row>
+    <row r="40" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AA40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC40" s="4"/>
+      <c r="AD40" s="5"/>
+      <c r="AE40" s="6"/>
+    </row>
+    <row r="41" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="5"/>
+      <c r="AE41" s="6"/>
+    </row>
+    <row r="42" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="6"/>
+    </row>
+    <row r="43" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AB43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2401,13 +2509,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
dynamic weighting for damage strategy
</commit_message>
<xml_diff>
--- a/strategies.xlsx
+++ b/strategies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="350">
   <si>
     <t>dist full x2</t>
   </si>
@@ -817,6 +817,255 @@
   </si>
   <si>
     <t>658+17</t>
+  </si>
+  <si>
+    <t>(0.5,0.75)</t>
+  </si>
+  <si>
+    <t>1294+16</t>
+  </si>
+  <si>
+    <t>596+13</t>
+  </si>
+  <si>
+    <t>662+13</t>
+  </si>
+  <si>
+    <t>1329+14</t>
+  </si>
+  <si>
+    <t>537+6</t>
+  </si>
+  <si>
+    <t>681+9</t>
+  </si>
+  <si>
+    <t>2956+83</t>
+  </si>
+  <si>
+    <t>796+14</t>
+  </si>
+  <si>
+    <t>horr. Time</t>
+  </si>
+  <si>
+    <t>prunning on, dyamic B (B, B/3), ThresholdSpeed</t>
+  </si>
+  <si>
+    <t>B=0.25, TS = 0.8</t>
+  </si>
+  <si>
+    <t>B=0.5, TS = 0.8</t>
+  </si>
+  <si>
+    <t>B=0.75, TS = 0.8</t>
+  </si>
+  <si>
+    <t>B*dam_full + (1-B)*dist</t>
+  </si>
+  <si>
+    <t>1304+18</t>
+  </si>
+  <si>
+    <t>634+11</t>
+  </si>
+  <si>
+    <t>654+7</t>
+  </si>
+  <si>
+    <t>1359+15</t>
+  </si>
+  <si>
+    <t>635+5</t>
+  </si>
+  <si>
+    <t>621+8</t>
+  </si>
+  <si>
+    <t>1425+32</t>
+  </si>
+  <si>
+    <t>668+11</t>
+  </si>
+  <si>
+    <t>592+7</t>
+  </si>
+  <si>
+    <t>B=0.25, TS = 0.6</t>
+  </si>
+  <si>
+    <t>B=0.5, TS = 0.6</t>
+  </si>
+  <si>
+    <t>B=0.75, TS = 0.6</t>
+  </si>
+  <si>
+    <t>1308+12</t>
+  </si>
+  <si>
+    <t>626+10</t>
+  </si>
+  <si>
+    <t>660+70</t>
+  </si>
+  <si>
+    <t>1454++40</t>
+  </si>
+  <si>
+    <t>653+7</t>
+  </si>
+  <si>
+    <t>614+11</t>
+  </si>
+  <si>
+    <t>B=0.25, TS = 1.0</t>
+  </si>
+  <si>
+    <t>B=0.5, TS = 1.0</t>
+  </si>
+  <si>
+    <t>B=0.75, TS = 1.0</t>
+  </si>
+  <si>
+    <t>1595+42</t>
+  </si>
+  <si>
+    <t>711+12</t>
+  </si>
+  <si>
+    <t>591+7</t>
+  </si>
+  <si>
+    <t>1309+18</t>
+  </si>
+  <si>
+    <t>632+11</t>
+  </si>
+  <si>
+    <t>650+10</t>
+  </si>
+  <si>
+    <t>1351+20</t>
+  </si>
+  <si>
+    <t>633+6</t>
+  </si>
+  <si>
+    <t>631+7</t>
+  </si>
+  <si>
+    <t>1451+30</t>
+  </si>
+  <si>
+    <t>663+10</t>
+  </si>
+  <si>
+    <t>590+7</t>
+  </si>
+  <si>
+    <t>1295+12</t>
+  </si>
+  <si>
+    <t>638+12</t>
+  </si>
+  <si>
+    <t>658+12</t>
+  </si>
+  <si>
+    <t>1357+17</t>
+  </si>
+  <si>
+    <t>622+9</t>
+  </si>
+  <si>
+    <t>646+9</t>
+  </si>
+  <si>
+    <t>(0.25,0.75)</t>
+  </si>
+  <si>
+    <t>1364+13</t>
+  </si>
+  <si>
+    <t>639+12</t>
+  </si>
+  <si>
+    <t>612+7</t>
+  </si>
+  <si>
+    <t>1475+35</t>
+  </si>
+  <si>
+    <t>663+9</t>
+  </si>
+  <si>
+    <t>605+8</t>
+  </si>
+  <si>
+    <t>1303+18</t>
+  </si>
+  <si>
+    <t>636+10</t>
+  </si>
+  <si>
+    <t>676+8</t>
+  </si>
+  <si>
+    <t>1322+21</t>
+  </si>
+  <si>
+    <t>638+9</t>
+  </si>
+  <si>
+    <t>644+12</t>
+  </si>
+  <si>
+    <t>1357+23</t>
+  </si>
+  <si>
+    <t>637+8</t>
+  </si>
+  <si>
+    <t>636+11</t>
+  </si>
+  <si>
+    <t>1402+23</t>
+  </si>
+  <si>
+    <t>666+12</t>
+  </si>
+  <si>
+    <t>588+9</t>
+  </si>
+  <si>
+    <t>Dyn. Damage</t>
+  </si>
+  <si>
+    <t>(0.5,B=0.75, TS = 1.0)</t>
+  </si>
+  <si>
+    <t>1300+10</t>
+  </si>
+  <si>
+    <t>614+9</t>
+  </si>
+  <si>
+    <t>653+12</t>
+  </si>
+  <si>
+    <t>1366+28</t>
+  </si>
+  <si>
+    <t>548+5</t>
+  </si>
+  <si>
+    <t>1427+30</t>
+  </si>
+  <si>
+    <t>672+8</t>
+  </si>
+  <si>
+    <t>594+7</t>
   </si>
 </sst>
 </file>
@@ -1237,29 +1486,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF43"/>
+  <dimension ref="A1:AF54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+    <sheetView tabSelected="1" topLeftCell="U30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD50" sqref="AD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
     <col min="11" max="11" width="2.85546875" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="9.140625" style="1"/>
     <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="31" width="9.140625" style="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -2241,9 +2493,21 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="O26" s="4"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="7"/>
+      <c r="E26" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>284</v>
+      </c>
       <c r="Z26" s="3" t="s">
         <v>112</v>
       </c>
@@ -2264,9 +2528,21 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="O27" s="4"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="7"/>
+      <c r="E27" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>287</v>
+      </c>
       <c r="Z27" s="2" t="s">
         <v>158</v>
       </c>
@@ -2284,9 +2560,18 @@
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="O28" s="4"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="7"/>
+      <c r="F28" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>290</v>
+      </c>
       <c r="AB28" s="1" t="s">
         <v>123</v>
       </c>
@@ -2304,9 +2589,19 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="O29" s="4"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="7"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="AB29" s="1" t="s">
         <v>150</v>
       </c>
@@ -2321,6 +2616,33 @@
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="W30" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="X30" s="6" t="s">
+        <v>317</v>
+      </c>
       <c r="AB30" s="1" t="s">
         <v>204</v>
       </c>
@@ -2335,6 +2657,31 @@
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F31" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V31" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="W31" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="X31" s="6" t="s">
+        <v>320</v>
+      </c>
       <c r="AB31" s="1" t="s">
         <v>205</v>
       </c>
@@ -2349,6 +2696,31 @@
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="N32" s="2"/>
+      <c r="U32" t="s">
+        <v>321</v>
+      </c>
+      <c r="V32" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="W32" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="X32" s="6" t="s">
+        <v>324</v>
+      </c>
       <c r="AB32" s="1" t="s">
         <v>206</v>
       </c>
@@ -2362,7 +2734,20 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="T33" s="1"/>
+      <c r="U33" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="X33" s="6" t="s">
+        <v>327</v>
+      </c>
       <c r="AA33" s="1" t="s">
         <v>124</v>
       </c>
@@ -2379,7 +2764,31 @@
         <v>219</v>
       </c>
     </row>
-    <row r="34" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="F34" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V34" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="W34" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="X34" s="6" t="s">
+        <v>330</v>
+      </c>
       <c r="AB34" s="1" t="s">
         <v>122</v>
       </c>
@@ -2393,7 +2802,31 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="F35" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="X35" s="6" t="s">
+        <v>333</v>
+      </c>
       <c r="AB35" s="1" t="s">
         <v>123</v>
       </c>
@@ -2410,7 +2843,31 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="U36" t="s">
+        <v>321</v>
+      </c>
+      <c r="V36" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="W36" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="X36" s="6" t="s">
+        <v>336</v>
+      </c>
       <c r="AB36" s="1" t="s">
         <v>150</v>
       </c>
@@ -2424,7 +2881,19 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="U37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V37" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="X37" s="6" t="s">
+        <v>339</v>
+      </c>
       <c r="AB37" s="1" t="s">
         <v>204</v>
       </c>
@@ -2438,7 +2907,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:32" x14ac:dyDescent="0.25">
       <c r="AB38" s="1" t="s">
         <v>205</v>
       </c>
@@ -2452,7 +2921,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:32" x14ac:dyDescent="0.25">
       <c r="AB39" s="1" t="s">
         <v>206</v>
       </c>
@@ -2466,40 +2935,172 @@
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="27:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:32" x14ac:dyDescent="0.25">
       <c r="AA40" s="1" t="s">
-        <v>140</v>
+        <v>267</v>
       </c>
       <c r="AB40" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AC40" s="4"/>
-      <c r="AD40" s="5"/>
-      <c r="AE40" s="6"/>
-    </row>
-    <row r="41" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AC40" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD40" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE40" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" spans="6:32" x14ac:dyDescent="0.25">
       <c r="AB41" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AC41" s="4"/>
-      <c r="AD41" s="5"/>
-      <c r="AE41" s="6"/>
-    </row>
-    <row r="42" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AC41" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD41" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="AE41" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="6:32" x14ac:dyDescent="0.25">
       <c r="AB42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AC42" s="4"/>
-      <c r="AD42" s="5"/>
-      <c r="AE42" s="6"/>
-    </row>
-    <row r="43" spans="27:32" x14ac:dyDescent="0.25">
+      <c r="AC42" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AD42" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE42" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="6:32" x14ac:dyDescent="0.25">
       <c r="AB43" s="1" t="s">
         <v>150</v>
       </c>
       <c r="AC43" s="4"/>
       <c r="AD43" s="5"/>
       <c r="AE43" s="6"/>
+    </row>
+    <row r="46" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="Z46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE46" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="Z47" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="Z48" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA48" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="AB48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC48" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD48" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="AE48" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="49" spans="26:31" x14ac:dyDescent="0.25">
+      <c r="Z49" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC49" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD49" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="AE49" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="26:31" x14ac:dyDescent="0.25">
+      <c r="Z50" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="AB50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC50" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD50" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="AE50" s="11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="51" spans="26:31" x14ac:dyDescent="0.25">
+      <c r="AB51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="5"/>
+      <c r="AE51" s="6"/>
+    </row>
+    <row r="52" spans="26:31" x14ac:dyDescent="0.25">
+      <c r="AB52" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="10"/>
+      <c r="AE52" s="11"/>
+    </row>
+    <row r="53" spans="26:31" x14ac:dyDescent="0.25">
+      <c r="AB53" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC53" s="9"/>
+      <c r="AD53" s="5"/>
+      <c r="AE53" s="11"/>
+    </row>
+    <row r="54" spans="26:31" x14ac:dyDescent="0.25">
+      <c r="AB54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="10"/>
+      <c r="AE54" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>